<commit_message>
API Auth, private repo
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -2368,52 +2368,38 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>.477</t>
+          <t>.473</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>.813</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>226</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>44</t>
-        </is>
-      </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
+          <t>.755</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>61</v>
+      </c>
+      <c r="F32" t="n">
+        <v>360</v>
+      </c>
+      <c r="G32" t="n">
+        <v>108</v>
+      </c>
+      <c r="H32" t="n">
+        <v>74</v>
+      </c>
+      <c r="I32" t="n">
+        <v>31</v>
+      </c>
+      <c r="J32" t="n">
+        <v>17</v>
+      </c>
+      <c r="K32" t="n">
+        <v>35</v>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>11/46</t>
+          <t>16/44</t>
         </is>
       </c>
     </row>
@@ -2430,52 +2416,38 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>.458</t>
+          <t>.472</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>.765</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>43</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
-      </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+          <t>.655</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>18</v>
+      </c>
+      <c r="F33" t="n">
+        <v>171</v>
+      </c>
+      <c r="G33" t="n">
+        <v>78</v>
+      </c>
+      <c r="H33" t="n">
+        <v>55</v>
+      </c>
+      <c r="I33" t="n">
+        <v>14</v>
+      </c>
+      <c r="J33" t="n">
+        <v>8</v>
+      </c>
+      <c r="K33" t="n">
+        <v>25</v>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>10/41</t>
+          <t>12/33</t>
         </is>
       </c>
     </row>
@@ -2492,52 +2464,38 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>.451</t>
+          <t>.452</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>.833</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>115</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
-      </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
+          <t>.814</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>29</v>
+      </c>
+      <c r="F34" t="n">
+        <v>196</v>
+      </c>
+      <c r="G34" t="n">
+        <v>68</v>
+      </c>
+      <c r="H34" t="n">
+        <v>51</v>
+      </c>
+      <c r="I34" t="n">
+        <v>16</v>
+      </c>
+      <c r="J34" t="n">
+        <v>6</v>
+      </c>
+      <c r="K34" t="n">
+        <v>36</v>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>10/44</t>
+          <t>14/38</t>
         </is>
       </c>
     </row>
@@ -2554,52 +2512,38 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>.476</t>
+          <t>.482</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>.800</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>193</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>44</t>
-        </is>
-      </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
+          <t>.797</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>31</v>
+      </c>
+      <c r="F35" t="n">
+        <v>290</v>
+      </c>
+      <c r="G35" t="n">
+        <v>82</v>
+      </c>
+      <c r="H35" t="n">
+        <v>71</v>
+      </c>
+      <c r="I35" t="n">
+        <v>22</v>
+      </c>
+      <c r="J35" t="n">
+        <v>13</v>
+      </c>
+      <c r="K35" t="n">
+        <v>34</v>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>12/39</t>
+          <t>15/36</t>
         </is>
       </c>
     </row>
@@ -2616,52 +2560,38 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>.500</t>
+          <t>.535</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>.647</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>118</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>46</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+          <t>.781</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>26</v>
+      </c>
+      <c r="F36" t="n">
+        <v>203</v>
+      </c>
+      <c r="G36" t="n">
+        <v>67</v>
+      </c>
+      <c r="H36" t="n">
+        <v>36</v>
+      </c>
+      <c r="I36" t="n">
+        <v>11</v>
+      </c>
+      <c r="J36" t="n">
+        <v>2</v>
+      </c>
+      <c r="K36" t="n">
+        <v>22</v>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>10/45</t>
+          <t>13/39</t>
         </is>
       </c>
     </row>
@@ -2678,52 +2608,38 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>.515</t>
+          <t>.504</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>.932</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>196</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>72</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>46</t>
-        </is>
-      </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>38</t>
-        </is>
+          <t>.896</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>32</v>
+      </c>
+      <c r="F37" t="n">
+        <v>326</v>
+      </c>
+      <c r="G37" t="n">
+        <v>110</v>
+      </c>
+      <c r="H37" t="n">
+        <v>86</v>
+      </c>
+      <c r="I37" t="n">
+        <v>19</v>
+      </c>
+      <c r="J37" t="n">
+        <v>16</v>
+      </c>
+      <c r="K37" t="n">
+        <v>57</v>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>13/44</t>
+          <t>17/40</t>
         </is>
       </c>
     </row>
@@ -2740,52 +2656,38 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>.512</t>
+          <t>.504</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>.698</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>221</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>71</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
+          <t>.700</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>25</v>
+      </c>
+      <c r="F38" t="n">
+        <v>304</v>
+      </c>
+      <c r="G38" t="n">
+        <v>112</v>
+      </c>
+      <c r="H38" t="n">
+        <v>40</v>
+      </c>
+      <c r="I38" t="n">
+        <v>25</v>
+      </c>
+      <c r="J38" t="n">
+        <v>8</v>
+      </c>
+      <c r="K38" t="n">
+        <v>33</v>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>12/41</t>
+          <t>14/36</t>
         </is>
       </c>
     </row>
@@ -2802,52 +2704,38 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>.509</t>
+          <t>.485</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>.759</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>207</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>83</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>38</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+          <t>.836</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>36</v>
+      </c>
+      <c r="F39" t="n">
+        <v>339</v>
+      </c>
+      <c r="G39" t="n">
+        <v>113</v>
+      </c>
+      <c r="H39" t="n">
+        <v>71</v>
+      </c>
+      <c r="I39" t="n">
+        <v>25</v>
+      </c>
+      <c r="J39" t="n">
+        <v>17</v>
+      </c>
+      <c r="K39" t="n">
+        <v>39</v>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>12/39</t>
+          <t>16/36</t>
         </is>
       </c>
     </row>
@@ -2864,52 +2752,38 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>.508</t>
+          <t>.469</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>.861</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>176</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>66</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>38</t>
-        </is>
-      </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+          <t>.873</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>22</v>
+      </c>
+      <c r="F40" t="n">
+        <v>266</v>
+      </c>
+      <c r="G40" t="n">
+        <v>116</v>
+      </c>
+      <c r="H40" t="n">
+        <v>66</v>
+      </c>
+      <c r="I40" t="n">
+        <v>18</v>
+      </c>
+      <c r="J40" t="n">
+        <v>14</v>
+      </c>
+      <c r="K40" t="n">
+        <v>41</v>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>11/42</t>
+          <t>15/35</t>
         </is>
       </c>
     </row>
@@ -2931,47 +2805,33 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>.821</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>233</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>61</t>
-        </is>
-      </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
+          <t>.793</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>48</v>
+      </c>
+      <c r="F41" t="n">
+        <v>375</v>
+      </c>
+      <c r="G41" t="n">
+        <v>100</v>
+      </c>
+      <c r="H41" t="n">
+        <v>82</v>
+      </c>
+      <c r="I41" t="n">
+        <v>29</v>
+      </c>
+      <c r="J41" t="n">
+        <v>14</v>
+      </c>
+      <c r="K41" t="n">
+        <v>42</v>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>11/43</t>
+          <t>18/43</t>
         </is>
       </c>
     </row>
@@ -3023,7 +2883,7 @@
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr">
         <is>
-          <t>0/30</t>
+          <t>0/24</t>
         </is>
       </c>
     </row>
@@ -3075,7 +2935,7 @@
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>0/29</t>
         </is>
       </c>
     </row>
@@ -3153,7 +3013,7 @@
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr">
         <is>
-          <t>0/29</t>
+          <t>0/26</t>
         </is>
       </c>
     </row>
@@ -3205,7 +3065,7 @@
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr">
         <is>
-          <t>0/29</t>
+          <t>0/24</t>
         </is>
       </c>
     </row>
@@ -3309,7 +3169,7 @@
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr">
         <is>
-          <t>0/38</t>
+          <t>0/30</t>
         </is>
       </c>
     </row>
@@ -3387,7 +3247,7 @@
       <c r="K57" t="inlineStr"/>
       <c r="L57" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>0/28</t>
         </is>
       </c>
     </row>
@@ -3439,7 +3299,7 @@
       <c r="K59" t="inlineStr"/>
       <c r="L59" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/32</t>
         </is>
       </c>
     </row>
@@ -3491,7 +3351,7 @@
       <c r="K61" t="inlineStr"/>
       <c r="L61" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/28</t>
         </is>
       </c>
     </row>
@@ -3569,7 +3429,7 @@
       <c r="K64" t="inlineStr"/>
       <c r="L64" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/29</t>
         </is>
       </c>
     </row>
@@ -3647,7 +3507,7 @@
       <c r="K67" t="inlineStr"/>
       <c r="L67" t="inlineStr">
         <is>
-          <t>0/38</t>
+          <t>0/31</t>
         </is>
       </c>
     </row>
@@ -3699,7 +3559,7 @@
       <c r="K69" t="inlineStr"/>
       <c r="L69" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/31</t>
         </is>
       </c>
     </row>
@@ -3725,7 +3585,7 @@
       <c r="K70" t="inlineStr"/>
       <c r="L70" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/32</t>
         </is>
       </c>
     </row>
@@ -3829,7 +3689,7 @@
       <c r="K74" t="inlineStr"/>
       <c r="L74" t="inlineStr">
         <is>
-          <t>0/20</t>
+          <t>0/16</t>
         </is>
       </c>
     </row>
@@ -3907,7 +3767,7 @@
       <c r="K77" t="inlineStr"/>
       <c r="L77" t="inlineStr">
         <is>
-          <t>0/20</t>
+          <t>0/16</t>
         </is>
       </c>
     </row>
@@ -3933,7 +3793,7 @@
       <c r="K78" t="inlineStr"/>
       <c r="L78" t="inlineStr">
         <is>
-          <t>0/20</t>
+          <t>0/18</t>
         </is>
       </c>
     </row>
@@ -3959,7 +3819,7 @@
       <c r="K79" t="inlineStr"/>
       <c r="L79" t="inlineStr">
         <is>
-          <t>0/20</t>
+          <t>0/18</t>
         </is>
       </c>
     </row>
@@ -4089,7 +3949,7 @@
       <c r="K84" t="inlineStr"/>
       <c r="L84" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/30</t>
         </is>
       </c>
     </row>
@@ -4141,7 +4001,7 @@
       <c r="K86" t="inlineStr"/>
       <c r="L86" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/31</t>
         </is>
       </c>
     </row>
@@ -4167,7 +4027,7 @@
       <c r="K87" t="inlineStr"/>
       <c r="L87" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/29</t>
         </is>
       </c>
     </row>
@@ -4193,7 +4053,7 @@
       <c r="K88" t="inlineStr"/>
       <c r="L88" t="inlineStr">
         <is>
-          <t>0/27</t>
+          <t>0/24</t>
         </is>
       </c>
     </row>
@@ -4349,7 +4209,7 @@
       <c r="K94" t="inlineStr"/>
       <c r="L94" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/27</t>
         </is>
       </c>
     </row>
@@ -4375,7 +4235,7 @@
       <c r="K95" t="inlineStr"/>
       <c r="L95" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/30</t>
         </is>
       </c>
     </row>
@@ -4453,7 +4313,7 @@
       <c r="K98" t="inlineStr"/>
       <c r="L98" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/30</t>
         </is>
       </c>
     </row>
@@ -4479,7 +4339,7 @@
       <c r="K99" t="inlineStr"/>
       <c r="L99" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>0/27</t>
         </is>
       </c>
     </row>
@@ -4583,7 +4443,7 @@
       <c r="K103" t="inlineStr"/>
       <c r="L103" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/31</t>
         </is>
       </c>
     </row>
@@ -4609,7 +4469,7 @@
       <c r="K104" t="inlineStr"/>
       <c r="L104" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/29</t>
         </is>
       </c>
     </row>
@@ -4635,7 +4495,7 @@
       <c r="K105" t="inlineStr"/>
       <c r="L105" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/29</t>
         </is>
       </c>
     </row>
@@ -4791,7 +4651,7 @@
       <c r="K111" t="inlineStr"/>
       <c r="L111" t="inlineStr">
         <is>
-          <t>0/40</t>
+          <t>0/31</t>
         </is>
       </c>
     </row>
@@ -4843,7 +4703,7 @@
       <c r="K113" t="inlineStr"/>
       <c r="L113" t="inlineStr">
         <is>
-          <t>0/30</t>
+          <t>0/27</t>
         </is>
       </c>
     </row>
@@ -4869,7 +4729,7 @@
       <c r="K114" t="inlineStr"/>
       <c r="L114" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/28</t>
         </is>
       </c>
     </row>
@@ -4895,7 +4755,7 @@
       <c r="K115" t="inlineStr"/>
       <c r="L115" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/29</t>
         </is>
       </c>
     </row>
@@ -5025,7 +4885,7 @@
       <c r="K120" t="inlineStr"/>
       <c r="L120" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/32</t>
         </is>
       </c>
     </row>
@@ -5103,7 +4963,7 @@
       <c r="K123" t="inlineStr"/>
       <c r="L123" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>0/25</t>
         </is>
       </c>
     </row>
@@ -5129,7 +4989,7 @@
       <c r="K124" t="inlineStr"/>
       <c r="L124" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/26</t>
         </is>
       </c>
     </row>
@@ -5233,7 +5093,7 @@
       <c r="K128" t="inlineStr"/>
       <c r="L128" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/30</t>
         </is>
       </c>
     </row>
@@ -5285,7 +5145,7 @@
       <c r="K130" t="inlineStr"/>
       <c r="L130" t="inlineStr">
         <is>
-          <t>0/28</t>
+          <t>0/25</t>
         </is>
       </c>
     </row>
@@ -5363,7 +5223,7 @@
       <c r="K133" t="inlineStr"/>
       <c r="L133" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/26</t>
         </is>
       </c>
     </row>
@@ -5415,7 +5275,7 @@
       <c r="K135" t="inlineStr"/>
       <c r="L135" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -5493,7 +5353,7 @@
       <c r="K138" t="inlineStr"/>
       <c r="L138" t="inlineStr">
         <is>
-          <t>0/30</t>
+          <t>0/26</t>
         </is>
       </c>
     </row>
@@ -5545,7 +5405,7 @@
       <c r="K140" t="inlineStr"/>
       <c r="L140" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/28</t>
         </is>
       </c>
     </row>
@@ -5649,7 +5509,7 @@
       <c r="K144" t="inlineStr"/>
       <c r="L144" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/28</t>
         </is>
       </c>
     </row>
@@ -5727,7 +5587,7 @@
       <c r="K147" t="inlineStr"/>
       <c r="L147" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/30</t>
         </is>
       </c>
     </row>
@@ -5779,7 +5639,7 @@
       <c r="K149" t="inlineStr"/>
       <c r="L149" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/31</t>
         </is>
       </c>
     </row>
@@ -5831,7 +5691,7 @@
       <c r="K151" t="inlineStr"/>
       <c r="L151" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/29</t>
         </is>
       </c>
     </row>
@@ -5909,7 +5769,7 @@
       <c r="K154" t="inlineStr"/>
       <c r="L154" t="inlineStr">
         <is>
-          <t>0/43</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -5987,7 +5847,7 @@
       <c r="K157" t="inlineStr"/>
       <c r="L157" t="inlineStr">
         <is>
-          <t>0/44</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -6039,7 +5899,7 @@
       <c r="K159" t="inlineStr"/>
       <c r="L159" t="inlineStr">
         <is>
-          <t>0/39</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -6065,7 +5925,7 @@
       <c r="K160" t="inlineStr"/>
       <c r="L160" t="inlineStr">
         <is>
-          <t>0/42</t>
+          <t>0/38</t>
         </is>
       </c>
     </row>
@@ -6169,7 +6029,7 @@
       <c r="K164" t="inlineStr"/>
       <c r="L164" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/29</t>
         </is>
       </c>
     </row>
@@ -6247,7 +6107,7 @@
       <c r="K167" t="inlineStr"/>
       <c r="L167" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/29</t>
         </is>
       </c>
     </row>
@@ -6273,7 +6133,7 @@
       <c r="K168" t="inlineStr"/>
       <c r="L168" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/33</t>
         </is>
       </c>
     </row>
@@ -6299,7 +6159,7 @@
       <c r="K169" t="inlineStr"/>
       <c r="L169" t="inlineStr">
         <is>
-          <t>0/30</t>
+          <t>0/26</t>
         </is>
       </c>
     </row>
@@ -6429,7 +6289,7 @@
       <c r="K174" t="inlineStr"/>
       <c r="L174" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/27</t>
         </is>
       </c>
     </row>
@@ -6481,7 +6341,7 @@
       <c r="K176" t="inlineStr"/>
       <c r="L176" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/32</t>
         </is>
       </c>
     </row>
@@ -6507,7 +6367,7 @@
       <c r="K177" t="inlineStr"/>
       <c r="L177" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/27</t>
         </is>
       </c>
     </row>
@@ -6533,7 +6393,7 @@
       <c r="K178" t="inlineStr"/>
       <c r="L178" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>0/28</t>
         </is>
       </c>
     </row>
@@ -6689,7 +6549,7 @@
       <c r="K184" t="inlineStr"/>
       <c r="L184" t="inlineStr">
         <is>
-          <t>0/38</t>
+          <t>0/31</t>
         </is>
       </c>
     </row>
@@ -6715,7 +6575,7 @@
       <c r="K185" t="inlineStr"/>
       <c r="L185" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -6793,7 +6653,7 @@
       <c r="K188" t="inlineStr"/>
       <c r="L188" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>0/29</t>
         </is>
       </c>
     </row>
@@ -6819,7 +6679,7 @@
       <c r="K189" t="inlineStr"/>
       <c r="L189" t="inlineStr">
         <is>
-          <t>0/38</t>
+          <t>0/31</t>
         </is>
       </c>
     </row>
@@ -6923,7 +6783,7 @@
       <c r="K193" t="inlineStr"/>
       <c r="L193" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/30</t>
         </is>
       </c>
     </row>
@@ -6949,7 +6809,7 @@
       <c r="K194" t="inlineStr"/>
       <c r="L194" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/28</t>
         </is>
       </c>
     </row>
@@ -6975,7 +6835,7 @@
       <c r="K195" t="inlineStr"/>
       <c r="L195" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/30</t>
         </is>
       </c>
     </row>
@@ -7131,7 +6991,7 @@
       <c r="K201" t="inlineStr"/>
       <c r="L201" t="inlineStr">
         <is>
-          <t>0/38</t>
+          <t>0/31</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
restore to previous version
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -3084,7 +3084,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>.434</t>
+          <t>.436</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3099,7 +3099,7 @@
         <v>237</v>
       </c>
       <c r="G44" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H44" t="n">
         <v>74</v>
@@ -3108,10 +3108,10 @@
         <v>11</v>
       </c>
       <c r="J44" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K44" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L44" t="inlineStr">
         <is>
@@ -3132,7 +3132,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>.532</t>
+          <t>.529</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3180,7 +3180,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>.461</t>
+          <t>.463</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3195,7 +3195,7 @@
         <v>265</v>
       </c>
       <c r="G46" t="n">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H46" t="n">
         <v>96</v>
@@ -3228,7 +3228,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>.456</t>
+          <t>.460</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3243,7 +3243,7 @@
         <v>245</v>
       </c>
       <c r="G47" t="n">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H47" t="n">
         <v>72</v>
@@ -3329,17 +3329,17 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>.733</t>
+          <t>.728</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F49" t="n">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="G49" t="n">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H49" t="n">
         <v>93</v>
@@ -3351,7 +3351,7 @@
         <v>9</v>
       </c>
       <c r="K49" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L49" t="inlineStr">
         <is>
@@ -3372,19 +3372,19 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>.513</t>
+          <t>.509</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>.908</t>
+          <t>.922</t>
         </is>
       </c>
       <c r="E50" t="n">
         <v>50</v>
       </c>
       <c r="F50" t="n">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="G50" t="n">
         <v>87</v>

</xml_diff>

<commit_message>
app V2: add scatter plots for season averages, transpose 1st DF
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -2988,38 +2988,52 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>.438</t>
+          <t>.461</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>.825</t>
-        </is>
-      </c>
-      <c r="E42" t="n">
-        <v>28</v>
-      </c>
-      <c r="F42" t="n">
-        <v>251</v>
-      </c>
-      <c r="G42" t="n">
-        <v>93</v>
-      </c>
-      <c r="H42" t="n">
-        <v>40</v>
-      </c>
-      <c r="I42" t="n">
-        <v>13</v>
-      </c>
-      <c r="J42" t="n">
-        <v>13</v>
-      </c>
-      <c r="K42" t="n">
-        <v>29</v>
+          <t>.811</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>591</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>236</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>104</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>19/39</t>
+          <t>42/42</t>
         </is>
       </c>
     </row>
@@ -3036,38 +3050,52 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>.475</t>
+          <t>.468</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>.717</t>
-        </is>
-      </c>
-      <c r="E43" t="n">
-        <v>44</v>
-      </c>
-      <c r="F43" t="n">
-        <v>283</v>
-      </c>
-      <c r="G43" t="n">
-        <v>128</v>
-      </c>
-      <c r="H43" t="n">
-        <v>66</v>
-      </c>
-      <c r="I43" t="n">
-        <v>19</v>
-      </c>
-      <c r="J43" t="n">
-        <v>11</v>
-      </c>
-      <c r="K43" t="n">
-        <v>28</v>
+          <t>.734</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>639</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>271</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>142</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>19/40</t>
+          <t>42/42</t>
         </is>
       </c>
     </row>
@@ -3084,38 +3112,52 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>.436</t>
+          <t>.460</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>.738</t>
-        </is>
-      </c>
-      <c r="E44" t="n">
-        <v>19</v>
-      </c>
-      <c r="F44" t="n">
-        <v>237</v>
-      </c>
-      <c r="G44" t="n">
-        <v>105</v>
-      </c>
-      <c r="H44" t="n">
-        <v>74</v>
-      </c>
-      <c r="I44" t="n">
-        <v>11</v>
-      </c>
-      <c r="J44" t="n">
-        <v>11</v>
-      </c>
-      <c r="K44" t="n">
-        <v>33</v>
+          <t>.766</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>575</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>222</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>164</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>18/40</t>
+          <t>41/41</t>
         </is>
       </c>
     </row>
@@ -3132,38 +3174,52 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>.529</t>
+          <t>.510</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>.643</t>
-        </is>
-      </c>
-      <c r="E45" t="n">
-        <v>30</v>
-      </c>
-      <c r="F45" t="n">
-        <v>230</v>
-      </c>
-      <c r="G45" t="n">
-        <v>67</v>
-      </c>
-      <c r="H45" t="n">
-        <v>50</v>
-      </c>
-      <c r="I45" t="n">
-        <v>16</v>
-      </c>
-      <c r="J45" t="n">
-        <v>10</v>
-      </c>
-      <c r="K45" t="n">
-        <v>29</v>
+          <t>.738</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>613</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>191</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>117</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>15/31</t>
+          <t>40/40</t>
         </is>
       </c>
     </row>
@@ -3180,38 +3236,52 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>.463</t>
+          <t>.461</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>.723</t>
-        </is>
-      </c>
-      <c r="E46" t="n">
-        <v>29</v>
-      </c>
-      <c r="F46" t="n">
-        <v>265</v>
-      </c>
-      <c r="G46" t="n">
-        <v>112</v>
-      </c>
-      <c r="H46" t="n">
-        <v>96</v>
-      </c>
-      <c r="I46" t="n">
-        <v>20</v>
-      </c>
-      <c r="J46" t="n">
-        <v>5</v>
-      </c>
-      <c r="K46" t="n">
-        <v>36</v>
+          <t>.740</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>568</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>252</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>173</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>16/37</t>
+          <t>38/38</t>
         </is>
       </c>
     </row>
@@ -3228,38 +3298,52 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>.460</t>
+          <t>.441</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>.773</t>
-        </is>
-      </c>
-      <c r="E47" t="n">
-        <v>42</v>
-      </c>
-      <c r="F47" t="n">
-        <v>245</v>
-      </c>
-      <c r="G47" t="n">
-        <v>77</v>
-      </c>
-      <c r="H47" t="n">
-        <v>72</v>
-      </c>
-      <c r="I47" t="n">
-        <v>18</v>
-      </c>
-      <c r="J47" t="n">
-        <v>9</v>
-      </c>
-      <c r="K47" t="n">
-        <v>30</v>
+          <t>.835</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>95</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>613</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>195</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>154</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>17/34</t>
+          <t>41/41</t>
         </is>
       </c>
     </row>
@@ -3276,38 +3360,52 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>.429</t>
+          <t>.426</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>.837</t>
-        </is>
-      </c>
-      <c r="E48" t="n">
-        <v>30</v>
-      </c>
-      <c r="F48" t="n">
-        <v>206</v>
-      </c>
-      <c r="G48" t="n">
-        <v>91</v>
-      </c>
-      <c r="H48" t="n">
-        <v>54</v>
-      </c>
-      <c r="I48" t="n">
-        <v>22</v>
-      </c>
-      <c r="J48" t="n">
-        <v>13</v>
-      </c>
-      <c r="K48" t="n">
-        <v>33</v>
+          <t>.841</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>526</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>219</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>137</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>18/40</t>
+          <t>41/41</t>
         </is>
       </c>
     </row>
@@ -3324,38 +3422,52 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>.515</t>
+          <t>.502</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>.728</t>
-        </is>
-      </c>
-      <c r="E49" t="n">
-        <v>31</v>
-      </c>
-      <c r="F49" t="n">
-        <v>420</v>
-      </c>
-      <c r="G49" t="n">
-        <v>133</v>
-      </c>
-      <c r="H49" t="n">
-        <v>93</v>
-      </c>
-      <c r="I49" t="n">
-        <v>20</v>
-      </c>
-      <c r="J49" t="n">
-        <v>9</v>
-      </c>
-      <c r="K49" t="n">
-        <v>50</v>
+          <t>.770</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>961</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>309</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>117</t>
+        </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>18/44</t>
+          <t>46/46</t>
         </is>
       </c>
     </row>
@@ -3372,38 +3484,52 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>.509</t>
+          <t>.477</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>.922</t>
-        </is>
-      </c>
-      <c r="E50" t="n">
-        <v>50</v>
-      </c>
-      <c r="F50" t="n">
-        <v>335</v>
-      </c>
-      <c r="G50" t="n">
-        <v>87</v>
-      </c>
-      <c r="H50" t="n">
-        <v>77</v>
-      </c>
-      <c r="I50" t="n">
-        <v>17</v>
-      </c>
-      <c r="J50" t="n">
-        <v>9</v>
-      </c>
-      <c r="K50" t="n">
-        <v>35</v>
+          <t>.836</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>650</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>185</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>175</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>16/39</t>
+          <t>40/40</t>
         </is>
       </c>
     </row>
@@ -3420,38 +3546,52 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>.488</t>
+          <t>.473</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>.909</t>
-        </is>
-      </c>
-      <c r="E51" t="n">
-        <v>42</v>
-      </c>
-      <c r="F51" t="n">
-        <v>396</v>
-      </c>
-      <c r="G51" t="n">
-        <v>117</v>
-      </c>
-      <c r="H51" t="n">
-        <v>59</v>
-      </c>
-      <c r="I51" t="n">
-        <v>18</v>
-      </c>
-      <c r="J51" t="n">
-        <v>16</v>
-      </c>
-      <c r="K51" t="n">
-        <v>48</v>
+          <t>.872</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>727</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>243</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>21/36</t>
+          <t>40/40</t>
         </is>
       </c>
     </row>
@@ -3466,18 +3606,54 @@
           <t>6</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr"/>
-      <c r="D52" t="inlineStr"/>
-      <c r="E52" t="inlineStr"/>
-      <c r="F52" t="inlineStr"/>
-      <c r="G52" t="inlineStr"/>
-      <c r="H52" t="inlineStr"/>
-      <c r="I52" t="inlineStr"/>
-      <c r="J52" t="inlineStr"/>
-      <c r="K52" t="inlineStr"/>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>.462</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>.759</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>306</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>129</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>45/45</t>
         </is>
       </c>
     </row>
@@ -3492,18 +3668,54 @@
           <t>6</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr"/>
-      <c r="D53" t="inlineStr"/>
-      <c r="E53" t="inlineStr"/>
-      <c r="F53" t="inlineStr"/>
-      <c r="G53" t="inlineStr"/>
-      <c r="H53" t="inlineStr"/>
-      <c r="I53" t="inlineStr"/>
-      <c r="J53" t="inlineStr"/>
-      <c r="K53" t="inlineStr"/>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>.453</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>.889</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>636</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>195</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>194</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>42/42</t>
         </is>
       </c>
     </row>
@@ -3518,18 +3730,54 @@
           <t>6</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="inlineStr"/>
-      <c r="E54" t="inlineStr"/>
-      <c r="F54" t="inlineStr"/>
-      <c r="G54" t="inlineStr"/>
-      <c r="H54" t="inlineStr"/>
-      <c r="I54" t="inlineStr"/>
-      <c r="J54" t="inlineStr"/>
-      <c r="K54" t="inlineStr"/>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>.495</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>.797</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>715</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>339</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>189</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>0/38</t>
+          <t>47/47</t>
         </is>
       </c>
     </row>
@@ -3544,18 +3792,54 @@
           <t>6</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr"/>
-      <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr"/>
-      <c r="F55" t="inlineStr"/>
-      <c r="G55" t="inlineStr"/>
-      <c r="H55" t="inlineStr"/>
-      <c r="I55" t="inlineStr"/>
-      <c r="J55" t="inlineStr"/>
-      <c r="K55" t="inlineStr"/>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>.471</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>.838</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>104</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>868</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>268</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>166</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>104</t>
+        </is>
+      </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>44/44</t>
         </is>
       </c>
     </row>
@@ -3570,18 +3854,54 @@
           <t>6</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr"/>
-      <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr"/>
-      <c r="F56" t="inlineStr"/>
-      <c r="G56" t="inlineStr"/>
-      <c r="H56" t="inlineStr"/>
-      <c r="I56" t="inlineStr"/>
-      <c r="J56" t="inlineStr"/>
-      <c r="K56" t="inlineStr"/>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>.477</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>.908</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>592</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>233</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>167</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>0/38</t>
+          <t>44/44</t>
         </is>
       </c>
     </row>
@@ -3596,18 +3916,54 @@
           <t>6</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr"/>
-      <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr"/>
-      <c r="F57" t="inlineStr"/>
-      <c r="G57" t="inlineStr"/>
-      <c r="H57" t="inlineStr"/>
-      <c r="I57" t="inlineStr"/>
-      <c r="J57" t="inlineStr"/>
-      <c r="K57" t="inlineStr"/>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>.496</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>.801</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>745</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>221</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>211</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>0/31</t>
+          <t>41/41</t>
         </is>
       </c>
     </row>
@@ -3622,18 +3978,54 @@
           <t>6</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr"/>
-      <c r="D58" t="inlineStr"/>
-      <c r="E58" t="inlineStr"/>
-      <c r="F58" t="inlineStr"/>
-      <c r="G58" t="inlineStr"/>
-      <c r="H58" t="inlineStr"/>
-      <c r="I58" t="inlineStr"/>
-      <c r="J58" t="inlineStr"/>
-      <c r="K58" t="inlineStr"/>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>.497</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>.756</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>736</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>196</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>45/45</t>
         </is>
       </c>
     </row>
@@ -3648,18 +4040,54 @@
           <t>6</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr"/>
-      <c r="D59" t="inlineStr"/>
-      <c r="E59" t="inlineStr"/>
-      <c r="F59" t="inlineStr"/>
-      <c r="G59" t="inlineStr"/>
-      <c r="H59" t="inlineStr"/>
-      <c r="I59" t="inlineStr"/>
-      <c r="J59" t="inlineStr"/>
-      <c r="K59" t="inlineStr"/>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>.442</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>.735</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>565</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>212</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
+      </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>0/27</t>
+          <t>44/44</t>
         </is>
       </c>
     </row>
@@ -3674,18 +4102,54 @@
           <t>6</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr"/>
-      <c r="D60" t="inlineStr"/>
-      <c r="E60" t="inlineStr"/>
-      <c r="F60" t="inlineStr"/>
-      <c r="G60" t="inlineStr"/>
-      <c r="H60" t="inlineStr"/>
-      <c r="I60" t="inlineStr"/>
-      <c r="J60" t="inlineStr"/>
-      <c r="K60" t="inlineStr"/>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>.489</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>.781</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>784</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>281</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>104</t>
+        </is>
+      </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>42/42</t>
         </is>
       </c>
     </row>
@@ -3700,18 +4164,54 @@
           <t>6</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr"/>
-      <c r="E61" t="inlineStr"/>
-      <c r="F61" t="inlineStr"/>
-      <c r="G61" t="inlineStr"/>
-      <c r="H61" t="inlineStr"/>
-      <c r="I61" t="inlineStr"/>
-      <c r="J61" t="inlineStr"/>
-      <c r="K61" t="inlineStr"/>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>.468</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>.826</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>547</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>141</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>40/40</t>
         </is>
       </c>
     </row>
@@ -3726,18 +4226,40 @@
           <t>7</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr"/>
-      <c r="D62" t="inlineStr"/>
-      <c r="E62" t="inlineStr"/>
-      <c r="F62" t="inlineStr"/>
-      <c r="G62" t="inlineStr"/>
-      <c r="H62" t="inlineStr"/>
-      <c r="I62" t="inlineStr"/>
-      <c r="J62" t="inlineStr"/>
-      <c r="K62" t="inlineStr"/>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>.463</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>.850</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>104</v>
+      </c>
+      <c r="F62" t="n">
+        <v>694</v>
+      </c>
+      <c r="G62" t="n">
+        <v>267</v>
+      </c>
+      <c r="H62" t="n">
+        <v>170</v>
+      </c>
+      <c r="I62" t="n">
+        <v>68</v>
+      </c>
+      <c r="J62" t="n">
+        <v>46</v>
+      </c>
+      <c r="K62" t="n">
+        <v>84</v>
+      </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>51/69</t>
         </is>
       </c>
     </row>
@@ -3752,18 +4274,40 @@
           <t>7</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr"/>
-      <c r="D63" t="inlineStr"/>
-      <c r="E63" t="inlineStr"/>
-      <c r="F63" t="inlineStr"/>
-      <c r="G63" t="inlineStr"/>
-      <c r="H63" t="inlineStr"/>
-      <c r="I63" t="inlineStr"/>
-      <c r="J63" t="inlineStr"/>
-      <c r="K63" t="inlineStr"/>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>.476</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>.843</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>104</v>
+      </c>
+      <c r="F63" t="n">
+        <v>986</v>
+      </c>
+      <c r="G63" t="n">
+        <v>307</v>
+      </c>
+      <c r="H63" t="n">
+        <v>169</v>
+      </c>
+      <c r="I63" t="n">
+        <v>56</v>
+      </c>
+      <c r="J63" t="n">
+        <v>41</v>
+      </c>
+      <c r="K63" t="n">
+        <v>115</v>
+      </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>52/65</t>
         </is>
       </c>
     </row>
@@ -3778,18 +4322,40 @@
           <t>7</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr"/>
-      <c r="D64" t="inlineStr"/>
-      <c r="E64" t="inlineStr"/>
-      <c r="F64" t="inlineStr"/>
-      <c r="G64" t="inlineStr"/>
-      <c r="H64" t="inlineStr"/>
-      <c r="I64" t="inlineStr"/>
-      <c r="J64" t="inlineStr"/>
-      <c r="K64" t="inlineStr"/>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>.492</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>.796</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>63</v>
+      </c>
+      <c r="F64" t="n">
+        <v>696</v>
+      </c>
+      <c r="G64" t="n">
+        <v>310</v>
+      </c>
+      <c r="H64" t="n">
+        <v>168</v>
+      </c>
+      <c r="I64" t="n">
+        <v>41</v>
+      </c>
+      <c r="J64" t="n">
+        <v>45</v>
+      </c>
+      <c r="K64" t="n">
+        <v>106</v>
+      </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>51/66</t>
         </is>
       </c>
     </row>
@@ -3804,18 +4370,40 @@
           <t>7</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr"/>
-      <c r="D65" t="inlineStr"/>
-      <c r="E65" t="inlineStr"/>
-      <c r="F65" t="inlineStr"/>
-      <c r="G65" t="inlineStr"/>
-      <c r="H65" t="inlineStr"/>
-      <c r="I65" t="inlineStr"/>
-      <c r="J65" t="inlineStr"/>
-      <c r="K65" t="inlineStr"/>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>.499</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>.796</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>60</v>
+      </c>
+      <c r="F65" t="n">
+        <v>804</v>
+      </c>
+      <c r="G65" t="n">
+        <v>255</v>
+      </c>
+      <c r="H65" t="n">
+        <v>154</v>
+      </c>
+      <c r="I65" t="n">
+        <v>37</v>
+      </c>
+      <c r="J65" t="n">
+        <v>27</v>
+      </c>
+      <c r="K65" t="n">
+        <v>103</v>
+      </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>44/55</t>
         </is>
       </c>
     </row>
@@ -3830,18 +4418,40 @@
           <t>7</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr"/>
-      <c r="D66" t="inlineStr"/>
-      <c r="E66" t="inlineStr"/>
-      <c r="F66" t="inlineStr"/>
-      <c r="G66" t="inlineStr"/>
-      <c r="H66" t="inlineStr"/>
-      <c r="I66" t="inlineStr"/>
-      <c r="J66" t="inlineStr"/>
-      <c r="K66" t="inlineStr"/>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>.495</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>.801</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>95</v>
+      </c>
+      <c r="F66" t="n">
+        <v>884</v>
+      </c>
+      <c r="G66" t="n">
+        <v>315</v>
+      </c>
+      <c r="H66" t="n">
+        <v>204</v>
+      </c>
+      <c r="I66" t="n">
+        <v>58</v>
+      </c>
+      <c r="J66" t="n">
+        <v>23</v>
+      </c>
+      <c r="K66" t="n">
+        <v>112</v>
+      </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>51/64</t>
         </is>
       </c>
     </row>
@@ -3856,18 +4466,40 @@
           <t>7</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr"/>
-      <c r="D67" t="inlineStr"/>
-      <c r="E67" t="inlineStr"/>
-      <c r="F67" t="inlineStr"/>
-      <c r="G67" t="inlineStr"/>
-      <c r="H67" t="inlineStr"/>
-      <c r="I67" t="inlineStr"/>
-      <c r="J67" t="inlineStr"/>
-      <c r="K67" t="inlineStr"/>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>.478</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>.790</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>54</v>
+      </c>
+      <c r="F67" t="n">
+        <v>610</v>
+      </c>
+      <c r="G67" t="n">
+        <v>229</v>
+      </c>
+      <c r="H67" t="n">
+        <v>147</v>
+      </c>
+      <c r="I67" t="n">
+        <v>34</v>
+      </c>
+      <c r="J67" t="n">
+        <v>27</v>
+      </c>
+      <c r="K67" t="n">
+        <v>87</v>
+      </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>0/39</t>
+          <t>50/59</t>
         </is>
       </c>
     </row>
@@ -3882,18 +4514,40 @@
           <t>7</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr"/>
-      <c r="D68" t="inlineStr"/>
-      <c r="E68" t="inlineStr"/>
-      <c r="F68" t="inlineStr"/>
-      <c r="G68" t="inlineStr"/>
-      <c r="H68" t="inlineStr"/>
-      <c r="I68" t="inlineStr"/>
-      <c r="J68" t="inlineStr"/>
-      <c r="K68" t="inlineStr"/>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>.479</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>.743</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>73</v>
+      </c>
+      <c r="F68" t="n">
+        <v>745</v>
+      </c>
+      <c r="G68" t="n">
+        <v>323</v>
+      </c>
+      <c r="H68" t="n">
+        <v>223</v>
+      </c>
+      <c r="I68" t="n">
+        <v>52</v>
+      </c>
+      <c r="J68" t="n">
+        <v>24</v>
+      </c>
+      <c r="K68" t="n">
+        <v>98</v>
+      </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>49/64</t>
         </is>
       </c>
     </row>
@@ -3908,18 +4562,40 @@
           <t>7</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr"/>
-      <c r="D69" t="inlineStr"/>
-      <c r="E69" t="inlineStr"/>
-      <c r="F69" t="inlineStr"/>
-      <c r="G69" t="inlineStr"/>
-      <c r="H69" t="inlineStr"/>
-      <c r="I69" t="inlineStr"/>
-      <c r="J69" t="inlineStr"/>
-      <c r="K69" t="inlineStr"/>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>.474</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>.780</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>69</v>
+      </c>
+      <c r="F69" t="n">
+        <v>720</v>
+      </c>
+      <c r="G69" t="n">
+        <v>237</v>
+      </c>
+      <c r="H69" t="n">
+        <v>172</v>
+      </c>
+      <c r="I69" t="n">
+        <v>54</v>
+      </c>
+      <c r="J69" t="n">
+        <v>32</v>
+      </c>
+      <c r="K69" t="n">
+        <v>82</v>
+      </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>46/63</t>
         </is>
       </c>
     </row>
@@ -3934,18 +4610,40 @@
           <t>7</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr"/>
-      <c r="D70" t="inlineStr"/>
-      <c r="E70" t="inlineStr"/>
-      <c r="F70" t="inlineStr"/>
-      <c r="G70" t="inlineStr"/>
-      <c r="H70" t="inlineStr"/>
-      <c r="I70" t="inlineStr"/>
-      <c r="J70" t="inlineStr"/>
-      <c r="K70" t="inlineStr"/>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>.490</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>.749</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>109</v>
+      </c>
+      <c r="F70" t="n">
+        <v>907</v>
+      </c>
+      <c r="G70" t="n">
+        <v>286</v>
+      </c>
+      <c r="H70" t="n">
+        <v>187</v>
+      </c>
+      <c r="I70" t="n">
+        <v>70</v>
+      </c>
+      <c r="J70" t="n">
+        <v>24</v>
+      </c>
+      <c r="K70" t="n">
+        <v>100</v>
+      </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>0/28</t>
+          <t>51/61</t>
         </is>
       </c>
     </row>
@@ -3960,18 +4658,40 @@
           <t>7</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr"/>
-      <c r="E71" t="inlineStr"/>
-      <c r="F71" t="inlineStr"/>
-      <c r="G71" t="inlineStr"/>
-      <c r="H71" t="inlineStr"/>
-      <c r="I71" t="inlineStr"/>
-      <c r="J71" t="inlineStr"/>
-      <c r="K71" t="inlineStr"/>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>.469</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>.848</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>99</v>
+      </c>
+      <c r="F71" t="n">
+        <v>745</v>
+      </c>
+      <c r="G71" t="n">
+        <v>258</v>
+      </c>
+      <c r="H71" t="n">
+        <v>187</v>
+      </c>
+      <c r="I71" t="n">
+        <v>52</v>
+      </c>
+      <c r="J71" t="n">
+        <v>30</v>
+      </c>
+      <c r="K71" t="n">
+        <v>90</v>
+      </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>52/62</t>
         </is>
       </c>
     </row>
@@ -3997,7 +4717,7 @@
       <c r="K72" t="inlineStr"/>
       <c r="L72" t="inlineStr">
         <is>
-          <t>0/20</t>
+          <t>0/22</t>
         </is>
       </c>
     </row>
@@ -4023,7 +4743,7 @@
       <c r="K73" t="inlineStr"/>
       <c r="L73" t="inlineStr">
         <is>
-          <t>0/20</t>
+          <t>0/28</t>
         </is>
       </c>
     </row>
@@ -4049,7 +4769,7 @@
       <c r="K74" t="inlineStr"/>
       <c r="L74" t="inlineStr">
         <is>
-          <t>0/21</t>
+          <t>0/27</t>
         </is>
       </c>
     </row>
@@ -4075,7 +4795,7 @@
       <c r="K75" t="inlineStr"/>
       <c r="L75" t="inlineStr">
         <is>
-          <t>0/20</t>
+          <t>0/23</t>
         </is>
       </c>
     </row>
@@ -4101,7 +4821,7 @@
       <c r="K76" t="inlineStr"/>
       <c r="L76" t="inlineStr">
         <is>
-          <t>0/20</t>
+          <t>0/23</t>
         </is>
       </c>
     </row>
@@ -4127,7 +4847,7 @@
       <c r="K77" t="inlineStr"/>
       <c r="L77" t="inlineStr">
         <is>
-          <t>0/21</t>
+          <t>0/18</t>
         </is>
       </c>
     </row>
@@ -4153,7 +4873,7 @@
       <c r="K78" t="inlineStr"/>
       <c r="L78" t="inlineStr">
         <is>
-          <t>0/16</t>
+          <t>0/24</t>
         </is>
       </c>
     </row>
@@ -4179,7 +4899,7 @@
       <c r="K79" t="inlineStr"/>
       <c r="L79" t="inlineStr">
         <is>
-          <t>0/19</t>
+          <t>0/25</t>
         </is>
       </c>
     </row>
@@ -4205,7 +4925,7 @@
       <c r="K80" t="inlineStr"/>
       <c r="L80" t="inlineStr">
         <is>
-          <t>0/20</t>
+          <t>0/24</t>
         </is>
       </c>
     </row>
@@ -4231,7 +4951,7 @@
       <c r="K81" t="inlineStr"/>
       <c r="L81" t="inlineStr">
         <is>
-          <t>0/18</t>
+          <t>0/27</t>
         </is>
       </c>
     </row>
@@ -4257,7 +4977,7 @@
       <c r="K82" t="inlineStr"/>
       <c r="L82" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/37</t>
         </is>
       </c>
     </row>
@@ -4283,7 +5003,7 @@
       <c r="K83" t="inlineStr"/>
       <c r="L83" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -4309,7 +5029,7 @@
       <c r="K84" t="inlineStr"/>
       <c r="L84" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>0/33</t>
         </is>
       </c>
     </row>
@@ -4335,7 +5055,7 @@
       <c r="K85" t="inlineStr"/>
       <c r="L85" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -4361,7 +5081,7 @@
       <c r="K86" t="inlineStr"/>
       <c r="L86" t="inlineStr">
         <is>
-          <t>0/29</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -4387,7 +5107,7 @@
       <c r="K87" t="inlineStr"/>
       <c r="L87" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/29</t>
         </is>
       </c>
     </row>
@@ -4413,7 +5133,7 @@
       <c r="K88" t="inlineStr"/>
       <c r="L88" t="inlineStr">
         <is>
-          <t>0/28</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -4439,7 +5159,7 @@
       <c r="K89" t="inlineStr"/>
       <c r="L89" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -4465,7 +5185,7 @@
       <c r="K90" t="inlineStr"/>
       <c r="L90" t="inlineStr">
         <is>
-          <t>0/31</t>
+          <t>0/32</t>
         </is>
       </c>
     </row>
@@ -4491,7 +5211,7 @@
       <c r="K91" t="inlineStr"/>
       <c r="L91" t="inlineStr">
         <is>
-          <t>0/31</t>
+          <t>0/33</t>
         </is>
       </c>
     </row>
@@ -4543,7 +5263,7 @@
       <c r="K93" t="inlineStr"/>
       <c r="L93" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -4569,7 +5289,7 @@
       <c r="K94" t="inlineStr"/>
       <c r="L94" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -4595,7 +5315,7 @@
       <c r="K95" t="inlineStr"/>
       <c r="L95" t="inlineStr">
         <is>
-          <t>0/27</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -4621,7 +5341,7 @@
       <c r="K96" t="inlineStr"/>
       <c r="L96" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -4647,7 +5367,7 @@
       <c r="K97" t="inlineStr"/>
       <c r="L97" t="inlineStr">
         <is>
-          <t>0/30</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -4673,7 +5393,7 @@
       <c r="K98" t="inlineStr"/>
       <c r="L98" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -4699,7 +5419,7 @@
       <c r="K99" t="inlineStr"/>
       <c r="L99" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/27</t>
         </is>
       </c>
     </row>
@@ -4725,7 +5445,7 @@
       <c r="K100" t="inlineStr"/>
       <c r="L100" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/37</t>
         </is>
       </c>
     </row>
@@ -4751,7 +5471,7 @@
       <c r="K101" t="inlineStr"/>
       <c r="L101" t="inlineStr">
         <is>
-          <t>0/31</t>
+          <t>0/32</t>
         </is>
       </c>
     </row>
@@ -4803,7 +5523,7 @@
       <c r="K103" t="inlineStr"/>
       <c r="L103" t="inlineStr">
         <is>
-          <t>0/28</t>
+          <t>0/36</t>
         </is>
       </c>
     </row>
@@ -4829,7 +5549,7 @@
       <c r="K104" t="inlineStr"/>
       <c r="L104" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -4855,7 +5575,7 @@
       <c r="K105" t="inlineStr"/>
       <c r="L105" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -4881,7 +5601,7 @@
       <c r="K106" t="inlineStr"/>
       <c r="L106" t="inlineStr">
         <is>
-          <t>0/38</t>
+          <t>0/37</t>
         </is>
       </c>
     </row>
@@ -4907,7 +5627,7 @@
       <c r="K107" t="inlineStr"/>
       <c r="L107" t="inlineStr">
         <is>
-          <t>0/38</t>
+          <t>0/37</t>
         </is>
       </c>
     </row>
@@ -4933,7 +5653,7 @@
       <c r="K108" t="inlineStr"/>
       <c r="L108" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -4959,7 +5679,7 @@
       <c r="K109" t="inlineStr"/>
       <c r="L109" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>0/37</t>
         </is>
       </c>
     </row>
@@ -4985,7 +5705,7 @@
       <c r="K110" t="inlineStr"/>
       <c r="L110" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/38</t>
         </is>
       </c>
     </row>
@@ -5011,7 +5731,7 @@
       <c r="K111" t="inlineStr"/>
       <c r="L111" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/30</t>
         </is>
       </c>
     </row>
@@ -5037,7 +5757,7 @@
       <c r="K112" t="inlineStr"/>
       <c r="L112" t="inlineStr">
         <is>
-          <t>0/30</t>
+          <t>0/32</t>
         </is>
       </c>
     </row>
@@ -5063,7 +5783,7 @@
       <c r="K113" t="inlineStr"/>
       <c r="L113" t="inlineStr">
         <is>
-          <t>0/29</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -5089,7 +5809,7 @@
       <c r="K114" t="inlineStr"/>
       <c r="L114" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/32</t>
         </is>
       </c>
     </row>
@@ -5115,7 +5835,7 @@
       <c r="K115" t="inlineStr"/>
       <c r="L115" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/29</t>
         </is>
       </c>
     </row>
@@ -5141,7 +5861,7 @@
       <c r="K116" t="inlineStr"/>
       <c r="L116" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/36</t>
         </is>
       </c>
     </row>
@@ -5193,7 +5913,7 @@
       <c r="K118" t="inlineStr"/>
       <c r="L118" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -5245,7 +5965,7 @@
       <c r="K120" t="inlineStr"/>
       <c r="L120" t="inlineStr">
         <is>
-          <t>0/27</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -5271,7 +5991,7 @@
       <c r="K121" t="inlineStr"/>
       <c r="L121" t="inlineStr">
         <is>
-          <t>0/30</t>
+          <t>0/32</t>
         </is>
       </c>
     </row>
@@ -5297,7 +6017,7 @@
       <c r="K122" t="inlineStr"/>
       <c r="L122" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/33</t>
         </is>
       </c>
     </row>
@@ -5323,7 +6043,7 @@
       <c r="K123" t="inlineStr"/>
       <c r="L123" t="inlineStr">
         <is>
-          <t>0/30</t>
+          <t>0/26</t>
         </is>
       </c>
     </row>
@@ -5349,7 +6069,7 @@
       <c r="K124" t="inlineStr"/>
       <c r="L124" t="inlineStr">
         <is>
-          <t>0/31</t>
+          <t>0/33</t>
         </is>
       </c>
     </row>
@@ -5375,7 +6095,7 @@
       <c r="K125" t="inlineStr"/>
       <c r="L125" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -5427,7 +6147,7 @@
       <c r="K127" t="inlineStr"/>
       <c r="L127" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -5453,7 +6173,7 @@
       <c r="K128" t="inlineStr"/>
       <c r="L128" t="inlineStr">
         <is>
-          <t>0/29</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -5479,7 +6199,7 @@
       <c r="K129" t="inlineStr"/>
       <c r="L129" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>0/33</t>
         </is>
       </c>
     </row>
@@ -5505,7 +6225,7 @@
       <c r="K130" t="inlineStr"/>
       <c r="L130" t="inlineStr">
         <is>
-          <t>0/29</t>
+          <t>0/32</t>
         </is>
       </c>
     </row>
@@ -5531,7 +6251,7 @@
       <c r="K131" t="inlineStr"/>
       <c r="L131" t="inlineStr">
         <is>
-          <t>0/31</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -5557,7 +6277,7 @@
       <c r="K132" t="inlineStr"/>
       <c r="L132" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/33</t>
         </is>
       </c>
     </row>
@@ -5609,7 +6329,7 @@
       <c r="K134" t="inlineStr"/>
       <c r="L134" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -5635,7 +6355,7 @@
       <c r="K135" t="inlineStr"/>
       <c r="L135" t="inlineStr">
         <is>
-          <t>0/28</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -5661,7 +6381,7 @@
       <c r="K136" t="inlineStr"/>
       <c r="L136" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -5687,7 +6407,7 @@
       <c r="K137" t="inlineStr"/>
       <c r="L137" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/36</t>
         </is>
       </c>
     </row>
@@ -5765,7 +6485,7 @@
       <c r="K140" t="inlineStr"/>
       <c r="L140" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/26</t>
         </is>
       </c>
     </row>
@@ -5791,7 +6511,7 @@
       <c r="K141" t="inlineStr"/>
       <c r="L141" t="inlineStr">
         <is>
-          <t>0/28</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -5817,7 +6537,7 @@
       <c r="K142" t="inlineStr"/>
       <c r="L142" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/37</t>
         </is>
       </c>
     </row>
@@ -5843,7 +6563,7 @@
       <c r="K143" t="inlineStr"/>
       <c r="L143" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/36</t>
         </is>
       </c>
     </row>
@@ -5869,7 +6589,7 @@
       <c r="K144" t="inlineStr"/>
       <c r="L144" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/37</t>
         </is>
       </c>
     </row>
@@ -5895,7 +6615,7 @@
       <c r="K145" t="inlineStr"/>
       <c r="L145" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>0/37</t>
         </is>
       </c>
     </row>
@@ -5921,7 +6641,7 @@
       <c r="K146" t="inlineStr"/>
       <c r="L146" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/37</t>
         </is>
       </c>
     </row>
@@ -5973,7 +6693,7 @@
       <c r="K148" t="inlineStr"/>
       <c r="L148" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -5999,7 +6719,7 @@
       <c r="K149" t="inlineStr"/>
       <c r="L149" t="inlineStr">
         <is>
-          <t>0/30</t>
+          <t>0/36</t>
         </is>
       </c>
     </row>
@@ -6025,7 +6745,7 @@
       <c r="K150" t="inlineStr"/>
       <c r="L150" t="inlineStr">
         <is>
-          <t>0/40</t>
+          <t>0/41</t>
         </is>
       </c>
     </row>
@@ -6051,7 +6771,7 @@
       <c r="K151" t="inlineStr"/>
       <c r="L151" t="inlineStr">
         <is>
-          <t>0/38</t>
+          <t>0/30</t>
         </is>
       </c>
     </row>
@@ -6077,7 +6797,7 @@
       <c r="K152" t="inlineStr"/>
       <c r="L152" t="inlineStr">
         <is>
-          <t>0/44</t>
+          <t>0/45</t>
         </is>
       </c>
     </row>
@@ -6103,7 +6823,7 @@
       <c r="K153" t="inlineStr"/>
       <c r="L153" t="inlineStr">
         <is>
-          <t>0/41</t>
+          <t>0/46</t>
         </is>
       </c>
     </row>
@@ -6129,7 +6849,7 @@
       <c r="K154" t="inlineStr"/>
       <c r="L154" t="inlineStr">
         <is>
-          <t>0/41</t>
+          <t>0/42</t>
         </is>
       </c>
     </row>
@@ -6155,7 +6875,7 @@
       <c r="K155" t="inlineStr"/>
       <c r="L155" t="inlineStr">
         <is>
-          <t>0/41</t>
+          <t>0/39</t>
         </is>
       </c>
     </row>
@@ -6181,7 +6901,7 @@
       <c r="K156" t="inlineStr"/>
       <c r="L156" t="inlineStr">
         <is>
-          <t>0/44</t>
+          <t>0/43</t>
         </is>
       </c>
     </row>
@@ -6207,7 +6927,7 @@
       <c r="K157" t="inlineStr"/>
       <c r="L157" t="inlineStr">
         <is>
-          <t>0/43</t>
+          <t>0/36</t>
         </is>
       </c>
     </row>
@@ -6259,7 +6979,7 @@
       <c r="K159" t="inlineStr"/>
       <c r="L159" t="inlineStr">
         <is>
-          <t>0/38</t>
+          <t>0/45</t>
         </is>
       </c>
     </row>
@@ -6285,7 +7005,7 @@
       <c r="K160" t="inlineStr"/>
       <c r="L160" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/45</t>
         </is>
       </c>
     </row>
@@ -6311,7 +7031,7 @@
       <c r="K161" t="inlineStr"/>
       <c r="L161" t="inlineStr">
         <is>
-          <t>0/48</t>
+          <t>0/47</t>
         </is>
       </c>
     </row>
@@ -6337,7 +7057,7 @@
       <c r="K162" t="inlineStr"/>
       <c r="L162" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/37</t>
         </is>
       </c>
     </row>
@@ -6363,7 +7083,7 @@
       <c r="K163" t="inlineStr"/>
       <c r="L163" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/36</t>
         </is>
       </c>
     </row>
@@ -6389,7 +7109,7 @@
       <c r="K164" t="inlineStr"/>
       <c r="L164" t="inlineStr">
         <is>
-          <t>0/38</t>
+          <t>0/37</t>
         </is>
       </c>
     </row>
@@ -6441,7 +7161,7 @@
       <c r="K166" t="inlineStr"/>
       <c r="L166" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/38</t>
         </is>
       </c>
     </row>
@@ -6467,7 +7187,7 @@
       <c r="K167" t="inlineStr"/>
       <c r="L167" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/27</t>
         </is>
       </c>
     </row>
@@ -6493,7 +7213,7 @@
       <c r="K168" t="inlineStr"/>
       <c r="L168" t="inlineStr">
         <is>
-          <t>0/28</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -6519,7 +7239,7 @@
       <c r="K169" t="inlineStr"/>
       <c r="L169" t="inlineStr">
         <is>
-          <t>0/30</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -6545,7 +7265,7 @@
       <c r="K170" t="inlineStr"/>
       <c r="L170" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -6571,7 +7291,7 @@
       <c r="K171" t="inlineStr"/>
       <c r="L171" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>0/36</t>
         </is>
       </c>
     </row>
@@ -6597,7 +7317,7 @@
       <c r="K172" t="inlineStr"/>
       <c r="L172" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -6623,7 +7343,7 @@
       <c r="K173" t="inlineStr"/>
       <c r="L173" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -6649,7 +7369,7 @@
       <c r="K174" t="inlineStr"/>
       <c r="L174" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -6701,7 +7421,7 @@
       <c r="K176" t="inlineStr"/>
       <c r="L176" t="inlineStr">
         <is>
-          <t>0/29</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -6727,7 +7447,7 @@
       <c r="K177" t="inlineStr"/>
       <c r="L177" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/26</t>
         </is>
       </c>
     </row>
@@ -6753,7 +7473,7 @@
       <c r="K178" t="inlineStr"/>
       <c r="L178" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>0/36</t>
         </is>
       </c>
     </row>
@@ -6779,7 +7499,7 @@
       <c r="K179" t="inlineStr"/>
       <c r="L179" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/38</t>
         </is>
       </c>
     </row>
@@ -6805,7 +7525,7 @@
       <c r="K180" t="inlineStr"/>
       <c r="L180" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/38</t>
         </is>
       </c>
     </row>
@@ -6831,7 +7551,7 @@
       <c r="K181" t="inlineStr"/>
       <c r="L181" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -6909,7 +7629,7 @@
       <c r="K184" t="inlineStr"/>
       <c r="L184" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/38</t>
         </is>
       </c>
     </row>
@@ -6935,7 +7655,7 @@
       <c r="K185" t="inlineStr"/>
       <c r="L185" t="inlineStr">
         <is>
-          <t>0/28</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -6961,7 +7681,7 @@
       <c r="K186" t="inlineStr"/>
       <c r="L186" t="inlineStr">
         <is>
-          <t>0/42</t>
+          <t>0/40</t>
         </is>
       </c>
     </row>
@@ -6987,7 +7707,7 @@
       <c r="K187" t="inlineStr"/>
       <c r="L187" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -7013,7 +7733,7 @@
       <c r="K188" t="inlineStr"/>
       <c r="L188" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/36</t>
         </is>
       </c>
     </row>
@@ -7039,7 +7759,7 @@
       <c r="K189" t="inlineStr"/>
       <c r="L189" t="inlineStr">
         <is>
-          <t>0/39</t>
+          <t>0/30</t>
         </is>
       </c>
     </row>
@@ -7091,7 +7811,7 @@
       <c r="K191" t="inlineStr"/>
       <c r="L191" t="inlineStr">
         <is>
-          <t>0/39</t>
+          <t>0/36</t>
         </is>
       </c>
     </row>
@@ -7117,7 +7837,7 @@
       <c r="K192" t="inlineStr"/>
       <c r="L192" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -7143,7 +7863,7 @@
       <c r="K193" t="inlineStr"/>
       <c r="L193" t="inlineStr">
         <is>
-          <t>0/29</t>
+          <t>0/36</t>
         </is>
       </c>
     </row>
@@ -7195,7 +7915,7 @@
       <c r="K195" t="inlineStr"/>
       <c r="L195" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/38</t>
         </is>
       </c>
     </row>
@@ -7221,7 +7941,7 @@
       <c r="K196" t="inlineStr"/>
       <c r="L196" t="inlineStr">
         <is>
-          <t>0/29</t>
+          <t>0/33</t>
         </is>
       </c>
     </row>
@@ -7247,7 +7967,7 @@
       <c r="K197" t="inlineStr"/>
       <c r="L197" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/39</t>
         </is>
       </c>
     </row>
@@ -7299,7 +8019,7 @@
       <c r="K199" t="inlineStr"/>
       <c r="L199" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>0/36</t>
         </is>
       </c>
     </row>
@@ -7351,7 +8071,7 @@
       <c r="K201" t="inlineStr"/>
       <c r="L201" t="inlineStr">
         <is>
-          <t>0/39</t>
+          <t>0/30</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix min and max table
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -508,52 +508,52 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>.449</t>
+          <t>.444</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>.800</t>
+          <t>.776</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>62</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>609</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>195</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>115</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
           <t>24</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>208</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>76</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>12/38</t>
+          <t>40/40</t>
         </is>
       </c>
     </row>
@@ -570,59 +570,59 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>.468</t>
+          <t>.472</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>.797</t>
+          <t>.851</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>67</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>212</t>
+          <t>642</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>240</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>135</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>41</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>70</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>11/34</t>
+          <t>37/37</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GG no re</t>
+          <t>VJ's Generators ⚡️</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -632,52 +632,52 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>.483</t>
+          <t>.461</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>.702</t>
+          <t>.669</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>67</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>237</t>
+          <t>594</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>74</t>
+          <t>218</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
+          <t>119</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
           <t>38</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>24</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>56</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>12/36</t>
+          <t>36/36</t>
         </is>
       </c>
     </row>
@@ -694,52 +694,52 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>.511</t>
+          <t>.496</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>.782</t>
+          <t>.796</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>54</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>201</t>
+          <t>574</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
+          <t>191</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>159</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
           <t>65</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>12/34</t>
+          <t>35/35</t>
         </is>
       </c>
     </row>
@@ -756,59 +756,59 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>.468</t>
+          <t>.461</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>.667</t>
+          <t>.746</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>47</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>152</t>
+          <t>530</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>215</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>112</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>28</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>22</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>77</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>10/34</t>
+          <t>35/35</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Load Management Legends</t>
+          <t>Zero Fears</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -818,52 +818,52 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>.444</t>
+          <t>.489</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>.867</t>
+          <t>.841</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>668</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>194</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>129</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
           <t>16</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>170</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>90</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>10/32</t>
+          <t>33/33</t>
         </is>
       </c>
     </row>
@@ -880,52 +880,52 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>.529</t>
+          <t>.515</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>.755</t>
+          <t>.796</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>50</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>629</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>205</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>127</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>32</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>61</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>11/30</t>
+          <t>34/34</t>
         </is>
       </c>
     </row>
@@ -942,52 +942,52 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>.496</t>
+          <t>.489</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>.773</t>
+          <t>.798</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>62</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>194</t>
+          <t>509</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>168</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>92</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>41</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>22</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>62</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>12/32</t>
+          <t>32/32</t>
         </is>
       </c>
     </row>
@@ -1004,52 +1004,52 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>.485</t>
+          <t>.471</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>.717</t>
+          <t>.795</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>25</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>146</t>
+          <t>437</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>138</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>92</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>20</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>61</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>8/22</t>
+          <t>23/23</t>
         </is>
       </c>
     </row>
@@ -1066,52 +1066,52 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>.527</t>
+          <t>.506</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>.810</t>
+          <t>.785</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>49</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>629</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>86</t>
+          <t>213</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>94</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>31</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>40</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>78</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>12/34</t>
+          <t>34/34</t>
         </is>
       </c>
     </row>
@@ -1126,18 +1126,54 @@
           <t>2</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>.496</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>.853</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>616</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>189</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>131</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>48/48</t>
         </is>
       </c>
     </row>
@@ -1152,25 +1188,61 @@
           <t>2</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>.457</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>.754</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>636</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>259</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>164</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>45/45</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>GG no re</t>
+          <t>VJ's Generators ⚡️</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1178,18 +1250,54 @@
           <t>2</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>.460</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>.789</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>753</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>219</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>171</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>44/44</t>
         </is>
       </c>
     </row>
@@ -1204,18 +1312,54 @@
           <t>2</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>.454</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>.800</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>576</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>179</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>0/29</t>
+          <t>37/37</t>
         </is>
       </c>
     </row>
@@ -1230,18 +1374,54 @@
           <t>2</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>.469</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>.841</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>616</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>206</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>179</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>0/30</t>
+          <t>39/39</t>
         </is>
       </c>
     </row>
@@ -1256,18 +1436,54 @@
           <t>2</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>.488</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>.828</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>86</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>820</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>243</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>191</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>0/31</t>
+          <t>43/43</t>
         </is>
       </c>
     </row>
@@ -1282,25 +1498,61 @@
           <t>2</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>.488</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>.819</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>836</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>276</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>181</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>45/45</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Load Management Legends</t>
+          <t>Zero Fears</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1308,18 +1560,54 @@
           <t>2</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>.503</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>.907</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>723</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>227</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>154</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>0/29</t>
+          <t>41/41</t>
         </is>
       </c>
     </row>
@@ -1334,18 +1622,54 @@
           <t>2</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>.486</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>.803</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>635</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>219</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>115</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>42/42</t>
         </is>
       </c>
     </row>
@@ -1360,18 +1684,54 @@
           <t>2</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>.485</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>.812</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>640</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>256</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>135</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>39/39</t>
         </is>
       </c>
     </row>
@@ -1386,18 +1746,40 @@
           <t>3</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>.532</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>.816</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>71</v>
+      </c>
+      <c r="F22" t="n">
+        <v>594</v>
+      </c>
+      <c r="G22" t="n">
+        <v>205</v>
+      </c>
+      <c r="H22" t="n">
+        <v>138</v>
+      </c>
+      <c r="I22" t="n">
+        <v>44</v>
+      </c>
+      <c r="J22" t="n">
+        <v>37</v>
+      </c>
+      <c r="K22" t="n">
+        <v>64</v>
+      </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>36/43</t>
         </is>
       </c>
     </row>
@@ -1412,25 +1794,47 @@
           <t>3</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>.472</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>.773</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>58</v>
+      </c>
+      <c r="F23" t="n">
+        <v>635</v>
+      </c>
+      <c r="G23" t="n">
+        <v>194</v>
+      </c>
+      <c r="H23" t="n">
+        <v>166</v>
+      </c>
+      <c r="I23" t="n">
+        <v>44</v>
+      </c>
+      <c r="J23" t="n">
+        <v>33</v>
+      </c>
+      <c r="K23" t="n">
+        <v>67</v>
+      </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>38/43</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>GG no re</t>
+          <t>VJ's Generators ⚡️</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1438,18 +1842,40 @@
           <t>3</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr"/>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>.482</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>.763</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>89</v>
+      </c>
+      <c r="F24" t="n">
+        <v>760</v>
+      </c>
+      <c r="G24" t="n">
+        <v>234</v>
+      </c>
+      <c r="H24" t="n">
+        <v>145</v>
+      </c>
+      <c r="I24" t="n">
+        <v>48</v>
+      </c>
+      <c r="J24" t="n">
+        <v>30</v>
+      </c>
+      <c r="K24" t="n">
+        <v>90</v>
+      </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>0/38</t>
+          <t>39/45</t>
         </is>
       </c>
     </row>
@@ -1464,18 +1890,40 @@
           <t>3</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
-      <c r="K25" t="inlineStr"/>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>.483</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>.830</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>63</v>
+      </c>
+      <c r="F25" t="n">
+        <v>515</v>
+      </c>
+      <c r="G25" t="n">
+        <v>190</v>
+      </c>
+      <c r="H25" t="n">
+        <v>81</v>
+      </c>
+      <c r="I25" t="n">
+        <v>31</v>
+      </c>
+      <c r="J25" t="n">
+        <v>16</v>
+      </c>
+      <c r="K25" t="n">
+        <v>54</v>
+      </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>37/44</t>
         </is>
       </c>
     </row>
@@ -1490,18 +1938,40 @@
           <t>3</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr"/>
-      <c r="K26" t="inlineStr"/>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>.454</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>.769</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>49</v>
+      </c>
+      <c r="F26" t="n">
+        <v>595</v>
+      </c>
+      <c r="G26" t="n">
+        <v>204</v>
+      </c>
+      <c r="H26" t="n">
+        <v>151</v>
+      </c>
+      <c r="I26" t="n">
+        <v>33</v>
+      </c>
+      <c r="J26" t="n">
+        <v>14</v>
+      </c>
+      <c r="K26" t="n">
+        <v>80</v>
+      </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>0/30</t>
+          <t>38/41</t>
         </is>
       </c>
     </row>
@@ -1516,18 +1986,40 @@
           <t>3</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
-      <c r="K27" t="inlineStr"/>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>.439</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>.825</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>27</v>
+      </c>
+      <c r="F27" t="n">
+        <v>417</v>
+      </c>
+      <c r="G27" t="n">
+        <v>141</v>
+      </c>
+      <c r="H27" t="n">
+        <v>130</v>
+      </c>
+      <c r="I27" t="n">
+        <v>29</v>
+      </c>
+      <c r="J27" t="n">
+        <v>16</v>
+      </c>
+      <c r="K27" t="n">
+        <v>67</v>
+      </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>0/28</t>
+          <t>30/33</t>
         </is>
       </c>
     </row>
@@ -1542,18 +2034,40 @@
           <t>3</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr"/>
-      <c r="K28" t="inlineStr"/>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>.486</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>.806</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>55</v>
+      </c>
+      <c r="F28" t="n">
+        <v>605</v>
+      </c>
+      <c r="G28" t="n">
+        <v>230</v>
+      </c>
+      <c r="H28" t="n">
+        <v>130</v>
+      </c>
+      <c r="I28" t="n">
+        <v>39</v>
+      </c>
+      <c r="J28" t="n">
+        <v>19</v>
+      </c>
+      <c r="K28" t="n">
+        <v>81</v>
+      </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>40/46</t>
         </is>
       </c>
     </row>
@@ -1568,25 +2082,47 @@
           <t>3</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr"/>
-      <c r="K29" t="inlineStr"/>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>.506</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>.867</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>81</v>
+      </c>
+      <c r="F29" t="n">
+        <v>701</v>
+      </c>
+      <c r="G29" t="n">
+        <v>198</v>
+      </c>
+      <c r="H29" t="n">
+        <v>157</v>
+      </c>
+      <c r="I29" t="n">
+        <v>57</v>
+      </c>
+      <c r="J29" t="n">
+        <v>15</v>
+      </c>
+      <c r="K29" t="n">
+        <v>91</v>
+      </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>43/45</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Load Management Legends</t>
+          <t>Zero Fears</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1594,18 +2130,40 @@
           <t>3</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr"/>
-      <c r="J30" t="inlineStr"/>
-      <c r="K30" t="inlineStr"/>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>.455</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>.829</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>42</v>
+      </c>
+      <c r="F30" t="n">
+        <v>565</v>
+      </c>
+      <c r="G30" t="n">
+        <v>216</v>
+      </c>
+      <c r="H30" t="n">
+        <v>124</v>
+      </c>
+      <c r="I30" t="n">
+        <v>45</v>
+      </c>
+      <c r="J30" t="n">
+        <v>17</v>
+      </c>
+      <c r="K30" t="n">
+        <v>80</v>
+      </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>43/46</t>
         </is>
       </c>
     </row>
@@ -1620,18 +2178,40 @@
           <t>3</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr"/>
-      <c r="K31" t="inlineStr"/>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>.481</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>.824</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>48</v>
+      </c>
+      <c r="F31" t="n">
+        <v>663</v>
+      </c>
+      <c r="G31" t="n">
+        <v>282</v>
+      </c>
+      <c r="H31" t="n">
+        <v>189</v>
+      </c>
+      <c r="I31" t="n">
+        <v>48</v>
+      </c>
+      <c r="J31" t="n">
+        <v>28</v>
+      </c>
+      <c r="K31" t="n">
+        <v>104</v>
+      </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>39/41</t>
         </is>
       </c>
     </row>
@@ -1657,7 +2237,7 @@
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/44</t>
         </is>
       </c>
     </row>
@@ -1690,7 +2270,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>GG no re</t>
+          <t>VJ's Generators ⚡️</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1709,14 +2289,14 @@
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>0/39</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Load Management Legends</t>
+          <t>Zero Fears</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1735,7 +2315,7 @@
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr">
         <is>
-          <t>0/38</t>
+          <t>0/43</t>
         </is>
       </c>
     </row>
@@ -1761,7 +2341,7 @@
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/38</t>
         </is>
       </c>
     </row>
@@ -1787,7 +2367,7 @@
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/43</t>
         </is>
       </c>
     </row>
@@ -1813,7 +2393,7 @@
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/43</t>
         </is>
       </c>
     </row>
@@ -1865,7 +2445,7 @@
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr">
         <is>
-          <t>0/25</t>
+          <t>0/23</t>
         </is>
       </c>
     </row>
@@ -1891,7 +2471,7 @@
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/42</t>
         </is>
       </c>
     </row>
@@ -1917,14 +2497,14 @@
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/36</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>GG no re</t>
+          <t>VJ's Generators ⚡️</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1943,7 +2523,7 @@
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/33</t>
         </is>
       </c>
     </row>
@@ -1969,14 +2549,14 @@
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr">
         <is>
-          <t>0/31</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Load Management Legends</t>
+          <t>Zero Fears</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1995,7 +2575,7 @@
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/43</t>
         </is>
       </c>
     </row>
@@ -2021,7 +2601,7 @@
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/33</t>
         </is>
       </c>
     </row>
@@ -2047,7 +2627,7 @@
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/30</t>
         </is>
       </c>
     </row>
@@ -2073,7 +2653,7 @@
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/33</t>
         </is>
       </c>
     </row>
@@ -2099,7 +2679,7 @@
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/49</t>
         </is>
       </c>
     </row>
@@ -2125,7 +2705,7 @@
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/41</t>
         </is>
       </c>
     </row>
@@ -2151,7 +2731,7 @@
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr">
         <is>
-          <t>0/27</t>
+          <t>0/24</t>
         </is>
       </c>
     </row>
@@ -2203,14 +2783,14 @@
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr">
         <is>
-          <t>0/29</t>
+          <t>0/32</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>GG no re</t>
+          <t>VJ's Generators ⚡️</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -2229,7 +2809,7 @@
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2835,7 @@
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr">
         <is>
-          <t>0/30</t>
+          <t>0/28</t>
         </is>
       </c>
     </row>
@@ -2281,7 +2861,7 @@
       <c r="K56" t="inlineStr"/>
       <c r="L56" t="inlineStr">
         <is>
-          <t>0/31</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -2314,7 +2894,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Load Management Legends</t>
+          <t>Zero Fears</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -2333,7 +2913,7 @@
       <c r="K58" t="inlineStr"/>
       <c r="L58" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/31</t>
         </is>
       </c>
     </row>
@@ -2359,7 +2939,7 @@
       <c r="K59" t="inlineStr"/>
       <c r="L59" t="inlineStr">
         <is>
-          <t>0/30</t>
+          <t>0/26</t>
         </is>
       </c>
     </row>
@@ -2385,7 +2965,7 @@
       <c r="K60" t="inlineStr"/>
       <c r="L60" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/32</t>
         </is>
       </c>
     </row>
@@ -2411,7 +2991,7 @@
       <c r="K61" t="inlineStr"/>
       <c r="L61" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/31</t>
         </is>
       </c>
     </row>
@@ -2437,7 +3017,7 @@
       <c r="K62" t="inlineStr"/>
       <c r="L62" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -2463,14 +3043,14 @@
       <c r="K63" t="inlineStr"/>
       <c r="L63" t="inlineStr">
         <is>
-          <t>0/27</t>
+          <t>0/25</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>GG no re</t>
+          <t>VJ's Generators ⚡️</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2489,7 +3069,7 @@
       <c r="K64" t="inlineStr"/>
       <c r="L64" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -2515,7 +3095,7 @@
       <c r="K65" t="inlineStr"/>
       <c r="L65" t="inlineStr">
         <is>
-          <t>0/40</t>
+          <t>0/36</t>
         </is>
       </c>
     </row>
@@ -2541,7 +3121,7 @@
       <c r="K66" t="inlineStr"/>
       <c r="L66" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/38</t>
         </is>
       </c>
     </row>
@@ -2567,14 +3147,14 @@
       <c r="K67" t="inlineStr"/>
       <c r="L67" t="inlineStr">
         <is>
-          <t>0/39</t>
+          <t>0/33</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Load Management Legends</t>
+          <t>Zero Fears</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2593,7 +3173,7 @@
       <c r="K68" t="inlineStr"/>
       <c r="L68" t="inlineStr">
         <is>
-          <t>0/38</t>
+          <t>0/39</t>
         </is>
       </c>
     </row>
@@ -2619,7 +3199,7 @@
       <c r="K69" t="inlineStr"/>
       <c r="L69" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/37</t>
         </is>
       </c>
     </row>
@@ -2645,7 +3225,7 @@
       <c r="K70" t="inlineStr"/>
       <c r="L70" t="inlineStr">
         <is>
-          <t>0/40</t>
+          <t>0/38</t>
         </is>
       </c>
     </row>
@@ -2671,7 +3251,7 @@
       <c r="K71" t="inlineStr"/>
       <c r="L71" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/36</t>
         </is>
       </c>
     </row>
@@ -2697,7 +3277,7 @@
       <c r="K72" t="inlineStr"/>
       <c r="L72" t="inlineStr">
         <is>
-          <t>0/3</t>
+          <t>0/2</t>
         </is>
       </c>
     </row>
@@ -2723,14 +3303,14 @@
       <c r="K73" t="inlineStr"/>
       <c r="L73" t="inlineStr">
         <is>
-          <t>0/3</t>
+          <t>0/2</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>GG no re</t>
+          <t>VJ's Generators ⚡️</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2749,7 +3329,7 @@
       <c r="K74" t="inlineStr"/>
       <c r="L74" t="inlineStr">
         <is>
-          <t>0/5</t>
+          <t>0/4</t>
         </is>
       </c>
     </row>
@@ -2827,7 +3407,7 @@
       <c r="K77" t="inlineStr"/>
       <c r="L77" t="inlineStr">
         <is>
-          <t>0/0</t>
+          <t>0/2</t>
         </is>
       </c>
     </row>
@@ -2879,14 +3459,14 @@
       <c r="K79" t="inlineStr"/>
       <c r="L79" t="inlineStr">
         <is>
-          <t>0/3</t>
+          <t>0/1</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Load Management Legends</t>
+          <t>Zero Fears</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2931,7 +3511,7 @@
       <c r="K81" t="inlineStr"/>
       <c r="L81" t="inlineStr">
         <is>
-          <t>0/0</t>
+          <t>0/1</t>
         </is>
       </c>
     </row>
@@ -2957,14 +3537,14 @@
       <c r="K82" t="inlineStr"/>
       <c r="L82" t="inlineStr">
         <is>
-          <t>0/24</t>
+          <t>0/22</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Load Management Legends</t>
+          <t>Zero Fears</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2990,7 +3570,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>GG no re</t>
+          <t>VJ's Generators ⚡️</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -3009,7 +3589,7 @@
       <c r="K84" t="inlineStr"/>
       <c r="L84" t="inlineStr">
         <is>
-          <t>0/23</t>
+          <t>0/24</t>
         </is>
       </c>
     </row>
@@ -3061,7 +3641,7 @@
       <c r="K86" t="inlineStr"/>
       <c r="L86" t="inlineStr">
         <is>
-          <t>0/21</t>
+          <t>0/23</t>
         </is>
       </c>
     </row>
@@ -3113,7 +3693,7 @@
       <c r="K88" t="inlineStr"/>
       <c r="L88" t="inlineStr">
         <is>
-          <t>0/22</t>
+          <t>0/20</t>
         </is>
       </c>
     </row>
@@ -3139,7 +3719,7 @@
       <c r="K89" t="inlineStr"/>
       <c r="L89" t="inlineStr">
         <is>
-          <t>0/25</t>
+          <t>0/24</t>
         </is>
       </c>
     </row>
@@ -3165,7 +3745,7 @@
       <c r="K90" t="inlineStr"/>
       <c r="L90" t="inlineStr">
         <is>
-          <t>0/25</t>
+          <t>0/24</t>
         </is>
       </c>
     </row>
@@ -3191,7 +3771,7 @@
       <c r="K91" t="inlineStr"/>
       <c r="L91" t="inlineStr">
         <is>
-          <t>0/18</t>
+          <t>0/17</t>
         </is>
       </c>
     </row>
@@ -3217,7 +3797,7 @@
       <c r="K92" t="inlineStr"/>
       <c r="L92" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -3243,14 +3823,14 @@
       <c r="K93" t="inlineStr"/>
       <c r="L93" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>0/33</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>GG no re</t>
+          <t>VJ's Generators ⚡️</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -3269,7 +3849,7 @@
       <c r="K94" t="inlineStr"/>
       <c r="L94" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/32</t>
         </is>
       </c>
     </row>
@@ -3295,7 +3875,7 @@
       <c r="K95" t="inlineStr"/>
       <c r="L95" t="inlineStr">
         <is>
-          <t>0/28</t>
+          <t>0/32</t>
         </is>
       </c>
     </row>
@@ -3321,14 +3901,14 @@
       <c r="K96" t="inlineStr"/>
       <c r="L96" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/32</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Load Management Legends</t>
+          <t>Zero Fears</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -3347,7 +3927,7 @@
       <c r="K97" t="inlineStr"/>
       <c r="L97" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -3373,7 +3953,7 @@
       <c r="K98" t="inlineStr"/>
       <c r="L98" t="inlineStr">
         <is>
-          <t>0/30</t>
+          <t>0/31</t>
         </is>
       </c>
     </row>
@@ -3399,7 +3979,7 @@
       <c r="K99" t="inlineStr"/>
       <c r="L99" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/32</t>
         </is>
       </c>
     </row>
@@ -3425,7 +4005,7 @@
       <c r="K100" t="inlineStr"/>
       <c r="L100" t="inlineStr">
         <is>
-          <t>0/28</t>
+          <t>0/24</t>
         </is>
       </c>
     </row>
@@ -3451,7 +4031,7 @@
       <c r="K101" t="inlineStr"/>
       <c r="L101" t="inlineStr">
         <is>
-          <t>0/31</t>
+          <t>0/33</t>
         </is>
       </c>
     </row>
@@ -3477,7 +4057,7 @@
       <c r="K102" t="inlineStr"/>
       <c r="L102" t="inlineStr">
         <is>
-          <t>0/38</t>
+          <t>0/39</t>
         </is>
       </c>
     </row>
@@ -3503,14 +4083,14 @@
       <c r="K103" t="inlineStr"/>
       <c r="L103" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/33</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>GG no re</t>
+          <t>VJ's Generators ⚡️</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -3529,7 +4109,7 @@
       <c r="K104" t="inlineStr"/>
       <c r="L104" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/38</t>
         </is>
       </c>
     </row>
@@ -3555,7 +4135,7 @@
       <c r="K105" t="inlineStr"/>
       <c r="L105" t="inlineStr">
         <is>
-          <t>0/29</t>
+          <t>0/24</t>
         </is>
       </c>
     </row>
@@ -3581,7 +4161,7 @@
       <c r="K106" t="inlineStr"/>
       <c r="L106" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/37</t>
         </is>
       </c>
     </row>
@@ -3607,7 +4187,7 @@
       <c r="K107" t="inlineStr"/>
       <c r="L107" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/39</t>
         </is>
       </c>
     </row>
@@ -3633,14 +4213,14 @@
       <c r="K108" t="inlineStr"/>
       <c r="L108" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/36</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Load Management Legends</t>
+          <t>Zero Fears</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -3659,7 +4239,7 @@
       <c r="K109" t="inlineStr"/>
       <c r="L109" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -3685,7 +4265,7 @@
       <c r="K110" t="inlineStr"/>
       <c r="L110" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -3711,7 +4291,7 @@
       <c r="K111" t="inlineStr"/>
       <c r="L111" t="inlineStr">
         <is>
-          <t>0/38</t>
+          <t>0/36</t>
         </is>
       </c>
     </row>
@@ -3737,7 +4317,7 @@
       <c r="K112" t="inlineStr"/>
       <c r="L112" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/39</t>
         </is>
       </c>
     </row>
@@ -3763,14 +4343,14 @@
       <c r="K113" t="inlineStr"/>
       <c r="L113" t="inlineStr">
         <is>
-          <t>0/39</t>
+          <t>0/38</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>GG no re</t>
+          <t>VJ's Generators ⚡️</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -3841,7 +4421,7 @@
       <c r="K116" t="inlineStr"/>
       <c r="L116" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/38</t>
         </is>
       </c>
     </row>
@@ -3867,7 +4447,7 @@
       <c r="K117" t="inlineStr"/>
       <c r="L117" t="inlineStr">
         <is>
-          <t>0/30</t>
+          <t>0/26</t>
         </is>
       </c>
     </row>
@@ -3919,14 +4499,14 @@
       <c r="K119" t="inlineStr"/>
       <c r="L119" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/39</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Load Management Legends</t>
+          <t>Zero Fears</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -3945,7 +4525,7 @@
       <c r="K120" t="inlineStr"/>
       <c r="L120" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/40</t>
         </is>
       </c>
     </row>
@@ -3971,7 +4551,7 @@
       <c r="K121" t="inlineStr"/>
       <c r="L121" t="inlineStr">
         <is>
-          <t>0/38</t>
+          <t>0/39</t>
         </is>
       </c>
     </row>
@@ -3997,7 +4577,7 @@
       <c r="K122" t="inlineStr"/>
       <c r="L122" t="inlineStr">
         <is>
-          <t>0/31</t>
+          <t>0/30</t>
         </is>
       </c>
     </row>
@@ -4023,14 +4603,14 @@
       <c r="K123" t="inlineStr"/>
       <c r="L123" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>GG no re</t>
+          <t>VJ's Generators ⚡️</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -4049,14 +4629,14 @@
       <c r="K124" t="inlineStr"/>
       <c r="L124" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/31</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Load Management Legends</t>
+          <t>Zero Fears</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -4075,7 +4655,7 @@
       <c r="K125" t="inlineStr"/>
       <c r="L125" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/36</t>
         </is>
       </c>
     </row>
@@ -4101,7 +4681,7 @@
       <c r="K126" t="inlineStr"/>
       <c r="L126" t="inlineStr">
         <is>
-          <t>0/31</t>
+          <t>0/33</t>
         </is>
       </c>
     </row>
@@ -4127,7 +4707,7 @@
       <c r="K127" t="inlineStr"/>
       <c r="L127" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/33</t>
         </is>
       </c>
     </row>
@@ -4153,7 +4733,7 @@
       <c r="K128" t="inlineStr"/>
       <c r="L128" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/26</t>
         </is>
       </c>
     </row>
@@ -4205,7 +4785,7 @@
       <c r="K130" t="inlineStr"/>
       <c r="L130" t="inlineStr">
         <is>
-          <t>0/25</t>
+          <t>0/22</t>
         </is>
       </c>
     </row>
@@ -4264,7 +4844,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>GG no re</t>
+          <t>VJ's Generators ⚡️</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -4309,14 +4889,14 @@
       <c r="K134" t="inlineStr"/>
       <c r="L134" t="inlineStr">
         <is>
-          <t>0/30</t>
+          <t>0/36</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Load Management Legends</t>
+          <t>Zero Fears</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -4335,7 +4915,7 @@
       <c r="K135" t="inlineStr"/>
       <c r="L135" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -4361,7 +4941,7 @@
       <c r="K136" t="inlineStr"/>
       <c r="L136" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/30</t>
         </is>
       </c>
     </row>
@@ -4387,7 +4967,7 @@
       <c r="K137" t="inlineStr"/>
       <c r="L137" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -4413,7 +4993,7 @@
       <c r="K138" t="inlineStr"/>
       <c r="L138" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/38</t>
         </is>
       </c>
     </row>
@@ -4439,7 +5019,7 @@
       <c r="K139" t="inlineStr"/>
       <c r="L139" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/39</t>
         </is>
       </c>
     </row>
@@ -4465,7 +5045,7 @@
       <c r="K140" t="inlineStr"/>
       <c r="L140" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/37</t>
         </is>
       </c>
     </row>
@@ -4491,7 +5071,7 @@
       <c r="K141" t="inlineStr"/>
       <c r="L141" t="inlineStr">
         <is>
-          <t>0/27</t>
+          <t>0/25</t>
         </is>
       </c>
     </row>
@@ -4517,7 +5097,7 @@
       <c r="K142" t="inlineStr"/>
       <c r="L142" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/38</t>
         </is>
       </c>
     </row>
@@ -4543,14 +5123,14 @@
       <c r="K143" t="inlineStr"/>
       <c r="L143" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>GG no re</t>
+          <t>VJ's Generators ⚡️</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -4595,7 +5175,7 @@
       <c r="K145" t="inlineStr"/>
       <c r="L145" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/33</t>
         </is>
       </c>
     </row>
@@ -4647,14 +5227,14 @@
       <c r="K147" t="inlineStr"/>
       <c r="L147" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/38</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Load Management Legends</t>
+          <t>Zero Fears</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4673,7 +5253,7 @@
       <c r="K148" t="inlineStr"/>
       <c r="L148" t="inlineStr">
         <is>
-          <t>0/34</t>
+          <t>0/36</t>
         </is>
       </c>
     </row>
@@ -4699,7 +5279,7 @@
       <c r="K149" t="inlineStr"/>
       <c r="L149" t="inlineStr">
         <is>
-          <t>0/30</t>
+          <t>0/26</t>
         </is>
       </c>
     </row>
@@ -4725,7 +5305,7 @@
       <c r="K150" t="inlineStr"/>
       <c r="L150" t="inlineStr">
         <is>
-          <t>0/38</t>
+          <t>0/37</t>
         </is>
       </c>
     </row>
@@ -4751,7 +5331,7 @@
       <c r="K151" t="inlineStr"/>
       <c r="L151" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/36</t>
         </is>
       </c>
     </row>
@@ -4777,7 +5357,7 @@
       <c r="K152" t="inlineStr"/>
       <c r="L152" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/31</t>
         </is>
       </c>
     </row>
@@ -4803,14 +5383,14 @@
       <c r="K153" t="inlineStr"/>
       <c r="L153" t="inlineStr">
         <is>
-          <t>0/28</t>
+          <t>0/23</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>GG no re</t>
+          <t>VJ's Generators ⚡️</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4829,7 +5409,7 @@
       <c r="K154" t="inlineStr"/>
       <c r="L154" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -4881,7 +5461,7 @@
       <c r="K156" t="inlineStr"/>
       <c r="L156" t="inlineStr">
         <is>
-          <t>0/29</t>
+          <t>0/33</t>
         </is>
       </c>
     </row>
@@ -4907,14 +5487,14 @@
       <c r="K157" t="inlineStr"/>
       <c r="L157" t="inlineStr">
         <is>
-          <t>0/31</t>
+          <t>0/27</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Load Management Legends</t>
+          <t>Zero Fears</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -4985,7 +5565,7 @@
       <c r="K160" t="inlineStr"/>
       <c r="L160" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/30</t>
         </is>
       </c>
     </row>
@@ -5011,7 +5591,7 @@
       <c r="K161" t="inlineStr"/>
       <c r="L161" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -5037,7 +5617,7 @@
       <c r="K162" t="inlineStr"/>
       <c r="L162" t="inlineStr">
         <is>
-          <t>0/44</t>
+          <t>0/48</t>
         </is>
       </c>
     </row>
@@ -5070,7 +5650,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>GG no re</t>
+          <t>VJ's Generators ⚡️</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -5089,7 +5669,7 @@
       <c r="K164" t="inlineStr"/>
       <c r="L164" t="inlineStr">
         <is>
-          <t>0/44</t>
+          <t>0/43</t>
         </is>
       </c>
     </row>
@@ -5115,7 +5695,7 @@
       <c r="K165" t="inlineStr"/>
       <c r="L165" t="inlineStr">
         <is>
-          <t>0/44</t>
+          <t>0/43</t>
         </is>
       </c>
     </row>
@@ -5141,7 +5721,7 @@
       <c r="K166" t="inlineStr"/>
       <c r="L166" t="inlineStr">
         <is>
-          <t>0/42</t>
+          <t>0/46</t>
         </is>
       </c>
     </row>
@@ -5167,7 +5747,7 @@
       <c r="K167" t="inlineStr"/>
       <c r="L167" t="inlineStr">
         <is>
-          <t>0/43</t>
+          <t>0/41</t>
         </is>
       </c>
     </row>
@@ -5193,7 +5773,7 @@
       <c r="K168" t="inlineStr"/>
       <c r="L168" t="inlineStr">
         <is>
-          <t>0/44</t>
+          <t>0/40</t>
         </is>
       </c>
     </row>
@@ -5219,14 +5799,14 @@
       <c r="K169" t="inlineStr"/>
       <c r="L169" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/30</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Load Management Legends</t>
+          <t>Zero Fears</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -5245,7 +5825,7 @@
       <c r="K170" t="inlineStr"/>
       <c r="L170" t="inlineStr">
         <is>
-          <t>0/44</t>
+          <t>0/43</t>
         </is>
       </c>
     </row>
@@ -5297,14 +5877,14 @@
       <c r="K172" t="inlineStr"/>
       <c r="L172" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/32</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Load Management Legends</t>
+          <t>Zero Fears</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -5323,14 +5903,14 @@
       <c r="K173" t="inlineStr"/>
       <c r="L173" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/32</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>GG no re</t>
+          <t>VJ's Generators ⚡️</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -5349,7 +5929,7 @@
       <c r="K174" t="inlineStr"/>
       <c r="L174" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/36</t>
         </is>
       </c>
     </row>
@@ -5375,7 +5955,7 @@
       <c r="K175" t="inlineStr"/>
       <c r="L175" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/30</t>
         </is>
       </c>
     </row>
@@ -5401,7 +5981,7 @@
       <c r="K176" t="inlineStr"/>
       <c r="L176" t="inlineStr">
         <is>
-          <t>0/30</t>
+          <t>0/32</t>
         </is>
       </c>
     </row>
@@ -5427,7 +6007,7 @@
       <c r="K177" t="inlineStr"/>
       <c r="L177" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/37</t>
         </is>
       </c>
     </row>
@@ -5453,7 +6033,7 @@
       <c r="K178" t="inlineStr"/>
       <c r="L178" t="inlineStr">
         <is>
-          <t>0/35</t>
+          <t>0/29</t>
         </is>
       </c>
     </row>
@@ -5505,7 +6085,7 @@
       <c r="K180" t="inlineStr"/>
       <c r="L180" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -5531,7 +6111,7 @@
       <c r="K181" t="inlineStr"/>
       <c r="L181" t="inlineStr">
         <is>
-          <t>0/26</t>
+          <t>0/23</t>
         </is>
       </c>
     </row>
@@ -5557,7 +6137,7 @@
       <c r="K182" t="inlineStr"/>
       <c r="L182" t="inlineStr">
         <is>
-          <t>0/32</t>
+          <t>0/34</t>
         </is>
       </c>
     </row>
@@ -5583,14 +6163,14 @@
       <c r="K183" t="inlineStr"/>
       <c r="L183" t="inlineStr">
         <is>
-          <t>0/37</t>
+          <t>0/33</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>GG no re</t>
+          <t>VJ's Generators ⚡️</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -5609,7 +6189,7 @@
       <c r="K184" t="inlineStr"/>
       <c r="L184" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -5635,7 +6215,7 @@
       <c r="K185" t="inlineStr"/>
       <c r="L185" t="inlineStr">
         <is>
-          <t>0/31</t>
+          <t>0/33</t>
         </is>
       </c>
     </row>
@@ -5661,14 +6241,14 @@
       <c r="K186" t="inlineStr"/>
       <c r="L186" t="inlineStr">
         <is>
-          <t>0/36</t>
+          <t>0/29</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>Load Management Legends</t>
+          <t>Zero Fears</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5739,7 +6319,7 @@
       <c r="K189" t="inlineStr"/>
       <c r="L189" t="inlineStr">
         <is>
-          <t>0/33</t>
+          <t>0/35</t>
         </is>
       </c>
     </row>
@@ -5765,7 +6345,7 @@
       <c r="K190" t="inlineStr"/>
       <c r="L190" t="inlineStr">
         <is>
-          <t>0/28</t>
+          <t>0/25</t>
         </is>
       </c>
     </row>

</xml_diff>